<commit_message>
copied files; editted node.js
</commit_message>
<xml_diff>
--- a/Database Spreadsheet Framework.xlsx
+++ b/Database Spreadsheet Framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\_Coding BootCamp\_weeks lessons\week 12\CMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\_Coding BootCamp\_weeks lessons\week 12\Employee_CMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F17F80-719F-4C75-B2B4-A54FB28335AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{106A6030-B0E8-4D59-962B-D86C62725052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2D9FE56-FE6A-40F4-9285-091278785816}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{C2D9FE56-FE6A-40F4-9285-091278785816}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>